<commit_message>
Student and Course Validation added
</commit_message>
<xml_diff>
--- a/resultFileInExcelFormat/CSE_101_Result.xlsx
+++ b/resultFileInExcelFormat/CSE_101_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIN TECHNOLOGY\Desktop\StudentResultManagementSystem\resultFileInExcelFormat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54EAF521-5E24-4129-A613-3A4C6FB118BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8755EF84-C754-47DD-98FB-C091D0FD7A11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -314,10 +314,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -415,188 +415,171 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B6" s="2">
         <v>60</v>
       </c>
       <c r="C6" s="3">
-        <v>25</v>
+        <v>26.5</v>
       </c>
       <c r="D6" s="3">
         <v>40</v>
       </c>
       <c r="E6" s="3">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B7" s="2">
         <v>60</v>
       </c>
       <c r="C7" s="3">
-        <v>26.5</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3">
         <v>40</v>
       </c>
       <c r="E7" s="3">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B8" s="2">
         <v>60</v>
       </c>
       <c r="C8" s="3">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <v>40</v>
       </c>
       <c r="E8" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B9" s="2">
         <v>60</v>
       </c>
       <c r="C9" s="3">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3">
         <v>40</v>
       </c>
       <c r="E9" s="3">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B10" s="2">
         <v>60</v>
       </c>
       <c r="C10" s="3">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3">
         <v>40</v>
       </c>
       <c r="E10" s="3">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B11" s="2">
         <v>60</v>
       </c>
       <c r="C11" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3">
         <v>40</v>
       </c>
       <c r="E11" s="3">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B12" s="2">
         <v>60</v>
       </c>
       <c r="C12" s="3">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3">
         <v>40</v>
       </c>
       <c r="E12" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B13" s="2">
         <v>60</v>
       </c>
       <c r="C13" s="3">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3">
         <v>40</v>
       </c>
       <c r="E13" s="3">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B14" s="2">
         <v>60</v>
       </c>
       <c r="C14" s="3">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D14" s="3">
         <v>40</v>
       </c>
       <c r="E14" s="3">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B15" s="2">
         <v>60</v>
       </c>
       <c r="C15" s="3">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D15" s="3">
         <v>40</v>
       </c>
       <c r="E15" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>615</v>
-      </c>
-      <c r="B16" s="2">
-        <v>60</v>
-      </c>
-      <c r="C16" s="3">
-        <v>44</v>
-      </c>
-      <c r="D16" s="3">
-        <v>40</v>
-      </c>
-      <c r="E16" s="3">
         <v>36</v>
       </c>
     </row>

</xml_diff>